<commit_message>
changes in the sheet and purchase and user controller
</commit_message>
<xml_diff>
--- a/updated_purchasedGoods.xlsx
+++ b/updated_purchasedGoods.xlsx
@@ -479,6 +479,7 @@
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H2" s="1"/>
       <c r="J2" s="1">
         <f>IF(F2&lt;&gt;"", "Kg CO2e/" &amp; F2, "")</f>
       </c>
@@ -498,6 +499,7 @@
       <c r="F3" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H3" s="1"/>
       <c r="J3" s="1">
         <f>IF(F3&lt;&gt;"", "Kg CO2e/" &amp; F3, "")</f>
       </c>
@@ -517,6 +519,7 @@
       <c r="F4" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H4" s="1"/>
       <c r="J4" s="1">
         <f>IF(F4&lt;&gt;"", "Kg CO2e/" &amp; F4, "")</f>
       </c>
@@ -528,6 +531,7 @@
       </c>
       <c r="C5" s="1"/>
       <c r="F5" s="1"/>
+      <c r="H5" s="1"/>
       <c r="J5" s="1">
         <f>IF(F5&lt;&gt;"", "Kg CO2e/" &amp; F5, "")</f>
       </c>
@@ -539,6 +543,7 @@
       </c>
       <c r="C6" s="1"/>
       <c r="F6" s="1"/>
+      <c r="H6" s="1"/>
       <c r="J6" s="1">
         <f>IF(F6&lt;&gt;"", "Kg CO2e/" &amp; F6, "")</f>
       </c>
@@ -550,6 +555,7 @@
       </c>
       <c r="C7" s="1"/>
       <c r="F7" s="1"/>
+      <c r="H7" s="1"/>
       <c r="J7" s="1">
         <f>IF(F7&lt;&gt;"", "Kg CO2e/" &amp; F7, "")</f>
       </c>
@@ -561,6 +567,7 @@
       </c>
       <c r="C8" s="1"/>
       <c r="F8" s="1"/>
+      <c r="H8" s="1"/>
       <c r="J8" s="1">
         <f>IF(F8&lt;&gt;"", "Kg CO2e/" &amp; F8, "")</f>
       </c>
@@ -572,6 +579,7 @@
       </c>
       <c r="C9" s="1"/>
       <c r="F9" s="1"/>
+      <c r="H9" s="1"/>
       <c r="J9" s="1">
         <f>IF(F9&lt;&gt;"", "Kg CO2e/" &amp; F9, "")</f>
       </c>
@@ -583,6 +591,7 @@
       </c>
       <c r="C10" s="1"/>
       <c r="F10" s="1"/>
+      <c r="H10" s="1"/>
       <c r="J10" s="1">
         <f>IF(F10&lt;&gt;"", "Kg CO2e/" &amp; F10, "")</f>
       </c>
@@ -594,6 +603,7 @@
       </c>
       <c r="C11" s="1"/>
       <c r="F11" s="1"/>
+      <c r="H11" s="1"/>
       <c r="J11" s="1">
         <f>IF(F11&lt;&gt;"", "Kg CO2e/" &amp; F11, "")</f>
       </c>
@@ -605,6 +615,7 @@
       </c>
       <c r="C12" s="1"/>
       <c r="F12" s="1"/>
+      <c r="H12" s="1"/>
       <c r="J12" s="1">
         <f>IF(F12&lt;&gt;"", "Kg CO2e/" &amp; F12, "")</f>
       </c>
@@ -616,6 +627,7 @@
       </c>
       <c r="C13" s="1"/>
       <c r="F13" s="1"/>
+      <c r="H13" s="1"/>
       <c r="J13" s="1">
         <f>IF(F13&lt;&gt;"", "Kg CO2e/" &amp; F13, "")</f>
       </c>
@@ -627,6 +639,7 @@
       </c>
       <c r="C14" s="1"/>
       <c r="F14" s="1"/>
+      <c r="H14" s="1"/>
       <c r="J14" s="1">
         <f>IF(F14&lt;&gt;"", "Kg CO2e/" &amp; F14, "")</f>
       </c>
@@ -638,6 +651,7 @@
       </c>
       <c r="C15" s="1"/>
       <c r="F15" s="1"/>
+      <c r="H15" s="1"/>
       <c r="J15" s="1">
         <f>IF(F15&lt;&gt;"", "Kg CO2e/" &amp; F15, "")</f>
       </c>
@@ -649,6 +663,7 @@
       </c>
       <c r="C16" s="1"/>
       <c r="F16" s="1"/>
+      <c r="H16" s="1"/>
       <c r="J16" s="1">
         <f>IF(F16&lt;&gt;"", "Kg CO2e/" &amp; F16, "")</f>
       </c>
@@ -660,6 +675,7 @@
       </c>
       <c r="C17" s="1"/>
       <c r="F17" s="1"/>
+      <c r="H17" s="1"/>
       <c r="J17" s="1">
         <f>IF(F17&lt;&gt;"", "Kg CO2e/" &amp; F17, "")</f>
       </c>
@@ -671,6 +687,7 @@
       </c>
       <c r="C18" s="1"/>
       <c r="F18" s="1"/>
+      <c r="H18" s="1"/>
       <c r="J18" s="1">
         <f>IF(F18&lt;&gt;"", "Kg CO2e/" &amp; F18, "")</f>
       </c>
@@ -682,6 +699,7 @@
       </c>
       <c r="C19" s="1"/>
       <c r="F19" s="1"/>
+      <c r="H19" s="1"/>
       <c r="J19" s="1">
         <f>IF(F19&lt;&gt;"", "Kg CO2e/" &amp; F19, "")</f>
       </c>
@@ -693,6 +711,7 @@
       </c>
       <c r="C20" s="1"/>
       <c r="F20" s="1"/>
+      <c r="H20" s="1"/>
       <c r="J20" s="1">
         <f>IF(F20&lt;&gt;"", "Kg CO2e/" &amp; F20, "")</f>
       </c>
@@ -704,6 +723,7 @@
       </c>
       <c r="C21" s="1"/>
       <c r="F21" s="1"/>
+      <c r="H21" s="1"/>
       <c r="J21" s="1">
         <f>IF(F21&lt;&gt;"", "Kg CO2e/" &amp; F21, "")</f>
       </c>
@@ -715,6 +735,7 @@
       </c>
       <c r="C22" s="1"/>
       <c r="F22" s="1"/>
+      <c r="H22" s="1"/>
       <c r="J22" s="1">
         <f>IF(F22&lt;&gt;"", "Kg CO2e/" &amp; F22, "")</f>
       </c>
@@ -726,6 +747,7 @@
       </c>
       <c r="C23" s="1"/>
       <c r="F23" s="1"/>
+      <c r="H23" s="1"/>
       <c r="J23" s="1">
         <f>IF(F23&lt;&gt;"", "Kg CO2e/" &amp; F23, "")</f>
       </c>
@@ -737,6 +759,7 @@
       </c>
       <c r="C24" s="1"/>
       <c r="F24" s="1"/>
+      <c r="H24" s="1"/>
       <c r="J24" s="1">
         <f>IF(F24&lt;&gt;"", "Kg CO2e/" &amp; F24, "")</f>
       </c>
@@ -748,6 +771,7 @@
       </c>
       <c r="C25" s="1"/>
       <c r="F25" s="1"/>
+      <c r="H25" s="1"/>
       <c r="J25" s="1">
         <f>IF(F25&lt;&gt;"", "Kg CO2e/" &amp; F25, "")</f>
       </c>
@@ -759,6 +783,7 @@
       </c>
       <c r="C26" s="1"/>
       <c r="F26" s="1"/>
+      <c r="H26" s="1"/>
       <c r="J26" s="1">
         <f>IF(F26&lt;&gt;"", "Kg CO2e/" &amp; F26, "")</f>
       </c>
@@ -770,6 +795,7 @@
       </c>
       <c r="C27" s="1"/>
       <c r="F27" s="1"/>
+      <c r="H27" s="1"/>
       <c r="J27" s="1">
         <f>IF(F27&lt;&gt;"", "Kg CO2e/" &amp; F27, "")</f>
       </c>
@@ -781,6 +807,7 @@
       </c>
       <c r="C28" s="1"/>
       <c r="F28" s="1"/>
+      <c r="H28" s="1"/>
       <c r="J28" s="1">
         <f>IF(F28&lt;&gt;"", "Kg CO2e/" &amp; F28, "")</f>
       </c>
@@ -792,6 +819,7 @@
       </c>
       <c r="C29" s="1"/>
       <c r="F29" s="1"/>
+      <c r="H29" s="1"/>
       <c r="J29" s="1">
         <f>IF(F29&lt;&gt;"", "Kg CO2e/" &amp; F29, "")</f>
       </c>
@@ -803,6 +831,7 @@
       </c>
       <c r="C30" s="1"/>
       <c r="F30" s="1"/>
+      <c r="H30" s="1"/>
       <c r="J30" s="1">
         <f>IF(F30&lt;&gt;"", "Kg CO2e/" &amp; F30, "")</f>
       </c>
@@ -814,6 +843,7 @@
       </c>
       <c r="C31" s="1"/>
       <c r="F31" s="1"/>
+      <c r="H31" s="1"/>
       <c r="J31" s="1">
         <f>IF(F31&lt;&gt;"", "Kg CO2e/" &amp; F31, "")</f>
       </c>
@@ -825,6 +855,7 @@
       </c>
       <c r="C32" s="1"/>
       <c r="F32" s="1"/>
+      <c r="H32" s="1"/>
       <c r="J32" s="1">
         <f>IF(F32&lt;&gt;"", "Kg CO2e/" &amp; F32, "")</f>
       </c>
@@ -836,6 +867,7 @@
       </c>
       <c r="C33" s="1"/>
       <c r="F33" s="1"/>
+      <c r="H33" s="1"/>
       <c r="J33" s="1">
         <f>IF(F33&lt;&gt;"", "Kg CO2e/" &amp; F33, "")</f>
       </c>
@@ -847,6 +879,7 @@
       </c>
       <c r="C34" s="1"/>
       <c r="F34" s="1"/>
+      <c r="H34" s="1"/>
       <c r="J34" s="1">
         <f>IF(F34&lt;&gt;"", "Kg CO2e/" &amp; F34, "")</f>
       </c>
@@ -858,6 +891,7 @@
       </c>
       <c r="C35" s="1"/>
       <c r="F35" s="1"/>
+      <c r="H35" s="1"/>
       <c r="J35" s="1">
         <f>IF(F35&lt;&gt;"", "Kg CO2e/" &amp; F35, "")</f>
       </c>
@@ -869,6 +903,7 @@
       </c>
       <c r="C36" s="1"/>
       <c r="F36" s="1"/>
+      <c r="H36" s="1"/>
       <c r="J36" s="1">
         <f>IF(F36&lt;&gt;"", "Kg CO2e/" &amp; F36, "")</f>
       </c>
@@ -880,6 +915,7 @@
       </c>
       <c r="C37" s="1"/>
       <c r="F37" s="1"/>
+      <c r="H37" s="1"/>
       <c r="J37" s="1">
         <f>IF(F37&lt;&gt;"", "Kg CO2e/" &amp; F37, "")</f>
       </c>
@@ -891,6 +927,7 @@
       </c>
       <c r="C38" s="1"/>
       <c r="F38" s="1"/>
+      <c r="H38" s="1"/>
       <c r="J38" s="1">
         <f>IF(F38&lt;&gt;"", "Kg CO2e/" &amp; F38, "")</f>
       </c>
@@ -902,6 +939,7 @@
       </c>
       <c r="C39" s="1"/>
       <c r="F39" s="1"/>
+      <c r="H39" s="1"/>
       <c r="J39" s="1">
         <f>IF(F39&lt;&gt;"", "Kg CO2e/" &amp; F39, "")</f>
       </c>
@@ -913,6 +951,7 @@
       </c>
       <c r="C40" s="1"/>
       <c r="F40" s="1"/>
+      <c r="H40" s="1"/>
       <c r="J40" s="1">
         <f>IF(F40&lt;&gt;"", "Kg CO2e/" &amp; F40, "")</f>
       </c>
@@ -924,6 +963,7 @@
       </c>
       <c r="C41" s="1"/>
       <c r="F41" s="1"/>
+      <c r="H41" s="1"/>
       <c r="J41" s="1">
         <f>IF(F41&lt;&gt;"", "Kg CO2e/" &amp; F41, "")</f>
       </c>
@@ -935,6 +975,7 @@
       </c>
       <c r="C42" s="1"/>
       <c r="F42" s="1"/>
+      <c r="H42" s="1"/>
       <c r="J42" s="1">
         <f>IF(F42&lt;&gt;"", "Kg CO2e/" &amp; F42, "")</f>
       </c>
@@ -946,6 +987,7 @@
       </c>
       <c r="C43" s="1"/>
       <c r="F43" s="1"/>
+      <c r="H43" s="1"/>
       <c r="J43" s="1">
         <f>IF(F43&lt;&gt;"", "Kg CO2e/" &amp; F43, "")</f>
       </c>
@@ -957,6 +999,7 @@
       </c>
       <c r="C44" s="1"/>
       <c r="F44" s="1"/>
+      <c r="H44" s="1"/>
       <c r="J44" s="1">
         <f>IF(F44&lt;&gt;"", "Kg CO2e/" &amp; F44, "")</f>
       </c>
@@ -968,6 +1011,7 @@
       </c>
       <c r="C45" s="1"/>
       <c r="F45" s="1"/>
+      <c r="H45" s="1"/>
       <c r="J45" s="1">
         <f>IF(F45&lt;&gt;"", "Kg CO2e/" &amp; F45, "")</f>
       </c>
@@ -979,6 +1023,7 @@
       </c>
       <c r="C46" s="1"/>
       <c r="F46" s="1"/>
+      <c r="H46" s="1"/>
       <c r="J46" s="1">
         <f>IF(F46&lt;&gt;"", "Kg CO2e/" &amp; F46, "")</f>
       </c>
@@ -990,6 +1035,7 @@
       </c>
       <c r="C47" s="1"/>
       <c r="F47" s="1"/>
+      <c r="H47" s="1"/>
       <c r="J47" s="1">
         <f>IF(F47&lt;&gt;"", "Kg CO2e/" &amp; F47, "")</f>
       </c>
@@ -1001,6 +1047,7 @@
       </c>
       <c r="C48" s="1"/>
       <c r="F48" s="1"/>
+      <c r="H48" s="1"/>
       <c r="J48" s="1">
         <f>IF(F48&lt;&gt;"", "Kg CO2e/" &amp; F48, "")</f>
       </c>
@@ -1012,6 +1059,7 @@
       </c>
       <c r="C49" s="1"/>
       <c r="F49" s="1"/>
+      <c r="H49" s="1"/>
       <c r="J49" s="1">
         <f>IF(F49&lt;&gt;"", "Kg CO2e/" &amp; F49, "")</f>
       </c>
@@ -1023,6 +1071,7 @@
       </c>
       <c r="C50" s="1"/>
       <c r="F50" s="1"/>
+      <c r="H50" s="1"/>
       <c r="J50" s="1">
         <f>IF(F50&lt;&gt;"", "Kg CO2e/" &amp; F50, "")</f>
       </c>
@@ -1034,6 +1083,7 @@
       </c>
       <c r="C51" s="1"/>
       <c r="F51" s="1"/>
+      <c r="H51" s="1"/>
       <c r="J51" s="1">
         <f>IF(F51&lt;&gt;"", "Kg CO2e/" &amp; F51, "")</f>
       </c>
@@ -1045,6 +1095,7 @@
       </c>
       <c r="C52" s="1"/>
       <c r="F52" s="1"/>
+      <c r="H52" s="1"/>
       <c r="J52" s="1">
         <f>IF(F52&lt;&gt;"", "Kg CO2e/" &amp; F52, "")</f>
       </c>
@@ -1056,6 +1107,7 @@
       </c>
       <c r="C53" s="1"/>
       <c r="F53" s="1"/>
+      <c r="H53" s="1"/>
       <c r="J53" s="1">
         <f>IF(F53&lt;&gt;"", "Kg CO2e/" &amp; F53, "")</f>
       </c>
@@ -1067,6 +1119,7 @@
       </c>
       <c r="C54" s="1"/>
       <c r="F54" s="1"/>
+      <c r="H54" s="1"/>
       <c r="J54" s="1">
         <f>IF(F54&lt;&gt;"", "Kg CO2e/" &amp; F54, "")</f>
       </c>
@@ -1078,6 +1131,7 @@
       </c>
       <c r="C55" s="1"/>
       <c r="F55" s="1"/>
+      <c r="H55" s="1"/>
       <c r="J55" s="1">
         <f>IF(F55&lt;&gt;"", "Kg CO2e/" &amp; F55, "")</f>
       </c>
@@ -1089,6 +1143,7 @@
       </c>
       <c r="C56" s="1"/>
       <c r="F56" s="1"/>
+      <c r="H56" s="1"/>
       <c r="J56" s="1">
         <f>IF(F56&lt;&gt;"", "Kg CO2e/" &amp; F56, "")</f>
       </c>
@@ -1100,6 +1155,7 @@
       </c>
       <c r="C57" s="1"/>
       <c r="F57" s="1"/>
+      <c r="H57" s="1"/>
       <c r="J57" s="1">
         <f>IF(F57&lt;&gt;"", "Kg CO2e/" &amp; F57, "")</f>
       </c>
@@ -1111,6 +1167,7 @@
       </c>
       <c r="C58" s="1"/>
       <c r="F58" s="1"/>
+      <c r="H58" s="1"/>
       <c r="J58" s="1">
         <f>IF(F58&lt;&gt;"", "Kg CO2e/" &amp; F58, "")</f>
       </c>
@@ -1122,6 +1179,7 @@
       </c>
       <c r="C59" s="1"/>
       <c r="F59" s="1"/>
+      <c r="H59" s="1"/>
       <c r="J59" s="1">
         <f>IF(F59&lt;&gt;"", "Kg CO2e/" &amp; F59, "")</f>
       </c>
@@ -1133,6 +1191,7 @@
       </c>
       <c r="C60" s="1"/>
       <c r="F60" s="1"/>
+      <c r="H60" s="1"/>
       <c r="J60" s="1">
         <f>IF(F60&lt;&gt;"", "Kg CO2e/" &amp; F60, "")</f>
       </c>
@@ -1144,6 +1203,7 @@
       </c>
       <c r="C61" s="1"/>
       <c r="F61" s="1"/>
+      <c r="H61" s="1"/>
       <c r="J61" s="1">
         <f>IF(F61&lt;&gt;"", "Kg CO2e/" &amp; F61, "")</f>
       </c>
@@ -1155,6 +1215,7 @@
       </c>
       <c r="C62" s="1"/>
       <c r="F62" s="1"/>
+      <c r="H62" s="1"/>
       <c r="J62" s="1">
         <f>IF(F62&lt;&gt;"", "Kg CO2e/" &amp; F62, "")</f>
       </c>
@@ -1166,6 +1227,7 @@
       </c>
       <c r="C63" s="1"/>
       <c r="F63" s="1"/>
+      <c r="H63" s="1"/>
       <c r="J63" s="1">
         <f>IF(F63&lt;&gt;"", "Kg CO2e/" &amp; F63, "")</f>
       </c>
@@ -1177,6 +1239,7 @@
       </c>
       <c r="C64" s="1"/>
       <c r="F64" s="1"/>
+      <c r="H64" s="1"/>
       <c r="J64" s="1">
         <f>IF(F64&lt;&gt;"", "Kg CO2e/" &amp; F64, "")</f>
       </c>
@@ -1188,6 +1251,7 @@
       </c>
       <c r="C65" s="1"/>
       <c r="F65" s="1"/>
+      <c r="H65" s="1"/>
       <c r="J65" s="1">
         <f>IF(F65&lt;&gt;"", "Kg CO2e/" &amp; F65, "")</f>
       </c>
@@ -1199,6 +1263,7 @@
       </c>
       <c r="C66" s="1"/>
       <c r="F66" s="1"/>
+      <c r="H66" s="1"/>
       <c r="J66" s="1">
         <f>IF(F66&lt;&gt;"", "Kg CO2e/" &amp; F66, "")</f>
       </c>
@@ -1210,6 +1275,7 @@
       </c>
       <c r="C67" s="1"/>
       <c r="F67" s="1"/>
+      <c r="H67" s="1"/>
       <c r="J67" s="1">
         <f>IF(F67&lt;&gt;"", "Kg CO2e/" &amp; F67, "")</f>
       </c>
@@ -1221,6 +1287,7 @@
       </c>
       <c r="C68" s="1"/>
       <c r="F68" s="1"/>
+      <c r="H68" s="1"/>
       <c r="J68" s="1">
         <f>IF(F68&lt;&gt;"", "Kg CO2e/" &amp; F68, "")</f>
       </c>
@@ -1232,6 +1299,7 @@
       </c>
       <c r="C69" s="1"/>
       <c r="F69" s="1"/>
+      <c r="H69" s="1"/>
       <c r="J69" s="1">
         <f>IF(F69&lt;&gt;"", "Kg CO2e/" &amp; F69, "")</f>
       </c>
@@ -1243,6 +1311,7 @@
       </c>
       <c r="C70" s="1"/>
       <c r="F70" s="1"/>
+      <c r="H70" s="1"/>
       <c r="J70" s="1">
         <f>IF(F70&lt;&gt;"", "Kg CO2e/" &amp; F70, "")</f>
       </c>
@@ -1254,6 +1323,7 @@
       </c>
       <c r="C71" s="1"/>
       <c r="F71" s="1"/>
+      <c r="H71" s="1"/>
       <c r="J71" s="1">
         <f>IF(F71&lt;&gt;"", "Kg CO2e/" &amp; F71, "")</f>
       </c>
@@ -1265,6 +1335,7 @@
       </c>
       <c r="C72" s="1"/>
       <c r="F72" s="1"/>
+      <c r="H72" s="1"/>
       <c r="J72" s="1">
         <f>IF(F72&lt;&gt;"", "Kg CO2e/" &amp; F72, "")</f>
       </c>
@@ -1276,6 +1347,7 @@
       </c>
       <c r="C73" s="1"/>
       <c r="F73" s="1"/>
+      <c r="H73" s="1"/>
       <c r="J73" s="1">
         <f>IF(F73&lt;&gt;"", "Kg CO2e/" &amp; F73, "")</f>
       </c>
@@ -1287,6 +1359,7 @@
       </c>
       <c r="C74" s="1"/>
       <c r="F74" s="1"/>
+      <c r="H74" s="1"/>
       <c r="J74" s="1">
         <f>IF(F74&lt;&gt;"", "Kg CO2e/" &amp; F74, "")</f>
       </c>
@@ -1298,6 +1371,7 @@
       </c>
       <c r="C75" s="1"/>
       <c r="F75" s="1"/>
+      <c r="H75" s="1"/>
       <c r="J75" s="1">
         <f>IF(F75&lt;&gt;"", "Kg CO2e/" &amp; F75, "")</f>
       </c>
@@ -1309,6 +1383,7 @@
       </c>
       <c r="C76" s="1"/>
       <c r="F76" s="1"/>
+      <c r="H76" s="1"/>
       <c r="J76" s="1">
         <f>IF(F76&lt;&gt;"", "Kg CO2e/" &amp; F76, "")</f>
       </c>
@@ -1320,6 +1395,7 @@
       </c>
       <c r="C77" s="1"/>
       <c r="F77" s="1"/>
+      <c r="H77" s="1"/>
       <c r="J77" s="1">
         <f>IF(F77&lt;&gt;"", "Kg CO2e/" &amp; F77, "")</f>
       </c>
@@ -1331,6 +1407,7 @@
       </c>
       <c r="C78" s="1"/>
       <c r="F78" s="1"/>
+      <c r="H78" s="1"/>
       <c r="J78" s="1">
         <f>IF(F78&lt;&gt;"", "Kg CO2e/" &amp; F78, "")</f>
       </c>
@@ -1342,6 +1419,7 @@
       </c>
       <c r="C79" s="1"/>
       <c r="F79" s="1"/>
+      <c r="H79" s="1"/>
       <c r="J79" s="1">
         <f>IF(F79&lt;&gt;"", "Kg CO2e/" &amp; F79, "")</f>
       </c>
@@ -1353,6 +1431,7 @@
       </c>
       <c r="C80" s="1"/>
       <c r="F80" s="1"/>
+      <c r="H80" s="1"/>
       <c r="J80" s="1">
         <f>IF(F80&lt;&gt;"", "Kg CO2e/" &amp; F80, "")</f>
       </c>
@@ -1364,6 +1443,7 @@
       </c>
       <c r="C81" s="1"/>
       <c r="F81" s="1"/>
+      <c r="H81" s="1"/>
       <c r="J81" s="1">
         <f>IF(F81&lt;&gt;"", "Kg CO2e/" &amp; F81, "")</f>
       </c>
@@ -1375,6 +1455,7 @@
       </c>
       <c r="C82" s="1"/>
       <c r="F82" s="1"/>
+      <c r="H82" s="1"/>
       <c r="J82" s="1">
         <f>IF(F82&lt;&gt;"", "Kg CO2e/" &amp; F82, "")</f>
       </c>
@@ -1386,6 +1467,7 @@
       </c>
       <c r="C83" s="1"/>
       <c r="F83" s="1"/>
+      <c r="H83" s="1"/>
       <c r="J83" s="1">
         <f>IF(F83&lt;&gt;"", "Kg CO2e/" &amp; F83, "")</f>
       </c>
@@ -1397,6 +1479,7 @@
       </c>
       <c r="C84" s="1"/>
       <c r="F84" s="1"/>
+      <c r="H84" s="1"/>
       <c r="J84" s="1">
         <f>IF(F84&lt;&gt;"", "Kg CO2e/" &amp; F84, "")</f>
       </c>
@@ -1408,6 +1491,7 @@
       </c>
       <c r="C85" s="1"/>
       <c r="F85" s="1"/>
+      <c r="H85" s="1"/>
       <c r="J85" s="1">
         <f>IF(F85&lt;&gt;"", "Kg CO2e/" &amp; F85, "")</f>
       </c>
@@ -1419,6 +1503,7 @@
       </c>
       <c r="C86" s="1"/>
       <c r="F86" s="1"/>
+      <c r="H86" s="1"/>
       <c r="J86" s="1">
         <f>IF(F86&lt;&gt;"", "Kg CO2e/" &amp; F86, "")</f>
       </c>
@@ -1430,6 +1515,7 @@
       </c>
       <c r="C87" s="1"/>
       <c r="F87" s="1"/>
+      <c r="H87" s="1"/>
       <c r="J87" s="1">
         <f>IF(F87&lt;&gt;"", "Kg CO2e/" &amp; F87, "")</f>
       </c>
@@ -1441,6 +1527,7 @@
       </c>
       <c r="C88" s="1"/>
       <c r="F88" s="1"/>
+      <c r="H88" s="1"/>
       <c r="J88" s="1">
         <f>IF(F88&lt;&gt;"", "Kg CO2e/" &amp; F88, "")</f>
       </c>
@@ -1452,6 +1539,7 @@
       </c>
       <c r="C89" s="1"/>
       <c r="F89" s="1"/>
+      <c r="H89" s="1"/>
       <c r="J89" s="1">
         <f>IF(F89&lt;&gt;"", "Kg CO2e/" &amp; F89, "")</f>
       </c>
@@ -1463,6 +1551,7 @@
       </c>
       <c r="C90" s="1"/>
       <c r="F90" s="1"/>
+      <c r="H90" s="1"/>
       <c r="J90" s="1">
         <f>IF(F90&lt;&gt;"", "Kg CO2e/" &amp; F90, "")</f>
       </c>
@@ -1474,6 +1563,7 @@
       </c>
       <c r="C91" s="1"/>
       <c r="F91" s="1"/>
+      <c r="H91" s="1"/>
       <c r="J91" s="1">
         <f>IF(F91&lt;&gt;"", "Kg CO2e/" &amp; F91, "")</f>
       </c>
@@ -1485,6 +1575,7 @@
       </c>
       <c r="C92" s="1"/>
       <c r="F92" s="1"/>
+      <c r="H92" s="1"/>
       <c r="J92" s="1">
         <f>IF(F92&lt;&gt;"", "Kg CO2e/" &amp; F92, "")</f>
       </c>
@@ -1496,6 +1587,7 @@
       </c>
       <c r="C93" s="1"/>
       <c r="F93" s="1"/>
+      <c r="H93" s="1"/>
       <c r="J93" s="1">
         <f>IF(F93&lt;&gt;"", "Kg CO2e/" &amp; F93, "")</f>
       </c>
@@ -1507,6 +1599,7 @@
       </c>
       <c r="C94" s="1"/>
       <c r="F94" s="1"/>
+      <c r="H94" s="1"/>
       <c r="J94" s="1">
         <f>IF(F94&lt;&gt;"", "Kg CO2e/" &amp; F94, "")</f>
       </c>
@@ -1518,6 +1611,7 @@
       </c>
       <c r="C95" s="1"/>
       <c r="F95" s="1"/>
+      <c r="H95" s="1"/>
       <c r="J95" s="1">
         <f>IF(F95&lt;&gt;"", "Kg CO2e/" &amp; F95, "")</f>
       </c>
@@ -1529,6 +1623,7 @@
       </c>
       <c r="C96" s="1"/>
       <c r="F96" s="1"/>
+      <c r="H96" s="1"/>
       <c r="J96" s="1">
         <f>IF(F96&lt;&gt;"", "Kg CO2e/" &amp; F96, "")</f>
       </c>
@@ -1540,6 +1635,7 @@
       </c>
       <c r="C97" s="1"/>
       <c r="F97" s="1"/>
+      <c r="H97" s="1"/>
       <c r="J97" s="1">
         <f>IF(F97&lt;&gt;"", "Kg CO2e/" &amp; F97, "")</f>
       </c>
@@ -1551,6 +1647,7 @@
       </c>
       <c r="C98" s="1"/>
       <c r="F98" s="1"/>
+      <c r="H98" s="1"/>
       <c r="J98" s="1">
         <f>IF(F98&lt;&gt;"", "Kg CO2e/" &amp; F98, "")</f>
       </c>
@@ -1562,6 +1659,7 @@
       </c>
       <c r="C99" s="1"/>
       <c r="F99" s="1"/>
+      <c r="H99" s="1"/>
       <c r="J99" s="1">
         <f>IF(F99&lt;&gt;"", "Kg CO2e/" &amp; F99, "")</f>
       </c>
@@ -1573,6 +1671,7 @@
       </c>
       <c r="C100" s="1"/>
       <c r="F100" s="1"/>
+      <c r="H100" s="1"/>
       <c r="J100" s="1">
         <f>IF(F100&lt;&gt;"", "Kg CO2e/" &amp; F100, "")</f>
       </c>
@@ -1584,6 +1683,7 @@
       </c>
       <c r="C101" s="1"/>
       <c r="F101" s="1"/>
+      <c r="H101" s="1"/>
       <c r="J101" s="1">
         <f>IF(F101&lt;&gt;"", "Kg CO2e/" &amp; F101, "")</f>
       </c>
@@ -1595,6 +1695,7 @@
       </c>
       <c r="C102" s="1"/>
       <c r="F102" s="1"/>
+      <c r="H102" s="1"/>
       <c r="J102" s="1">
         <f>IF(F102&lt;&gt;"", "Kg CO2e/" &amp; F102, "")</f>
       </c>
@@ -1606,6 +1707,7 @@
       </c>
       <c r="C103" s="1"/>
       <c r="F103" s="1"/>
+      <c r="H103" s="1"/>
       <c r="J103" s="1">
         <f>IF(F103&lt;&gt;"", "Kg CO2e/" &amp; F103, "")</f>
       </c>
@@ -1617,6 +1719,7 @@
       </c>
       <c r="C104" s="1"/>
       <c r="F104" s="1"/>
+      <c r="H104" s="1"/>
       <c r="J104" s="1">
         <f>IF(F104&lt;&gt;"", "Kg CO2e/" &amp; F104, "")</f>
       </c>
@@ -1628,6 +1731,7 @@
       </c>
       <c r="C105" s="1"/>
       <c r="F105" s="1"/>
+      <c r="H105" s="1"/>
       <c r="J105" s="1">
         <f>IF(F105&lt;&gt;"", "Kg CO2e/" &amp; F105, "")</f>
       </c>
@@ -1639,6 +1743,7 @@
       </c>
       <c r="C106" s="1"/>
       <c r="F106" s="1"/>
+      <c r="H106" s="1"/>
       <c r="J106" s="1">
         <f>IF(F106&lt;&gt;"", "Kg CO2e/" &amp; F106, "")</f>
       </c>
@@ -1650,6 +1755,7 @@
       </c>
       <c r="C107" s="1"/>
       <c r="F107" s="1"/>
+      <c r="H107" s="1"/>
       <c r="J107" s="1">
         <f>IF(F107&lt;&gt;"", "Kg CO2e/" &amp; F107, "")</f>
       </c>
@@ -1661,6 +1767,7 @@
       </c>
       <c r="C108" s="1"/>
       <c r="F108" s="1"/>
+      <c r="H108" s="1"/>
       <c r="J108" s="1">
         <f>IF(F108&lt;&gt;"", "Kg CO2e/" &amp; F108, "")</f>
       </c>
@@ -1672,6 +1779,7 @@
       </c>
       <c r="C109" s="1"/>
       <c r="F109" s="1"/>
+      <c r="H109" s="1"/>
       <c r="J109" s="1">
         <f>IF(F109&lt;&gt;"", "Kg CO2e/" &amp; F109, "")</f>
       </c>
@@ -1683,6 +1791,7 @@
       </c>
       <c r="C110" s="1"/>
       <c r="F110" s="1"/>
+      <c r="H110" s="1"/>
       <c r="J110" s="1">
         <f>IF(F110&lt;&gt;"", "Kg CO2e/" &amp; F110, "")</f>
       </c>
@@ -1694,6 +1803,7 @@
       </c>
       <c r="C111" s="1"/>
       <c r="F111" s="1"/>
+      <c r="H111" s="1"/>
       <c r="J111" s="1">
         <f>IF(F111&lt;&gt;"", "Kg CO2e/" &amp; F111, "")</f>
       </c>
@@ -1705,6 +1815,7 @@
       </c>
       <c r="C112" s="1"/>
       <c r="F112" s="1"/>
+      <c r="H112" s="1"/>
       <c r="J112" s="1">
         <f>IF(F112&lt;&gt;"", "Kg CO2e/" &amp; F112, "")</f>
       </c>
@@ -1716,6 +1827,7 @@
       </c>
       <c r="C113" s="1"/>
       <c r="F113" s="1"/>
+      <c r="H113" s="1"/>
       <c r="J113" s="1">
         <f>IF(F113&lt;&gt;"", "Kg CO2e/" &amp; F113, "")</f>
       </c>
@@ -1727,6 +1839,7 @@
       </c>
       <c r="C114" s="1"/>
       <c r="F114" s="1"/>
+      <c r="H114" s="1"/>
       <c r="J114" s="1">
         <f>IF(F114&lt;&gt;"", "Kg CO2e/" &amp; F114, "")</f>
       </c>
@@ -1738,6 +1851,7 @@
       </c>
       <c r="C115" s="1"/>
       <c r="F115" s="1"/>
+      <c r="H115" s="1"/>
       <c r="J115" s="1">
         <f>IF(F115&lt;&gt;"", "Kg CO2e/" &amp; F115, "")</f>
       </c>
@@ -1749,6 +1863,7 @@
       </c>
       <c r="C116" s="1"/>
       <c r="F116" s="1"/>
+      <c r="H116" s="1"/>
       <c r="J116" s="1">
         <f>IF(F116&lt;&gt;"", "Kg CO2e/" &amp; F116, "")</f>
       </c>
@@ -1760,6 +1875,7 @@
       </c>
       <c r="C117" s="1"/>
       <c r="F117" s="1"/>
+      <c r="H117" s="1"/>
       <c r="J117" s="1">
         <f>IF(F117&lt;&gt;"", "Kg CO2e/" &amp; F117, "")</f>
       </c>
@@ -1771,6 +1887,7 @@
       </c>
       <c r="C118" s="1"/>
       <c r="F118" s="1"/>
+      <c r="H118" s="1"/>
       <c r="J118" s="1">
         <f>IF(F118&lt;&gt;"", "Kg CO2e/" &amp; F118, "")</f>
       </c>
@@ -1782,6 +1899,7 @@
       </c>
       <c r="C119" s="1"/>
       <c r="F119" s="1"/>
+      <c r="H119" s="1"/>
       <c r="J119" s="1">
         <f>IF(F119&lt;&gt;"", "Kg CO2e/" &amp; F119, "")</f>
       </c>
@@ -1793,6 +1911,7 @@
       </c>
       <c r="C120" s="1"/>
       <c r="F120" s="1"/>
+      <c r="H120" s="1"/>
       <c r="J120" s="1">
         <f>IF(F120&lt;&gt;"", "Kg CO2e/" &amp; F120, "")</f>
       </c>
@@ -1804,6 +1923,7 @@
       </c>
       <c r="C121" s="1"/>
       <c r="F121" s="1"/>
+      <c r="H121" s="1"/>
       <c r="J121" s="1">
         <f>IF(F121&lt;&gt;"", "Kg CO2e/" &amp; F121, "")</f>
       </c>
@@ -1815,6 +1935,7 @@
       </c>
       <c r="C122" s="1"/>
       <c r="F122" s="1"/>
+      <c r="H122" s="1"/>
       <c r="J122" s="1">
         <f>IF(F122&lt;&gt;"", "Kg CO2e/" &amp; F122, "")</f>
       </c>
@@ -1826,6 +1947,7 @@
       </c>
       <c r="C123" s="1"/>
       <c r="F123" s="1"/>
+      <c r="H123" s="1"/>
       <c r="J123" s="1">
         <f>IF(F123&lt;&gt;"", "Kg CO2e/" &amp; F123, "")</f>
       </c>
@@ -1837,6 +1959,7 @@
       </c>
       <c r="C124" s="1"/>
       <c r="F124" s="1"/>
+      <c r="H124" s="1"/>
       <c r="J124" s="1">
         <f>IF(F124&lt;&gt;"", "Kg CO2e/" &amp; F124, "")</f>
       </c>
@@ -1848,6 +1971,7 @@
       </c>
       <c r="C125" s="1"/>
       <c r="F125" s="1"/>
+      <c r="H125" s="1"/>
       <c r="J125" s="1">
         <f>IF(F125&lt;&gt;"", "Kg CO2e/" &amp; F125, "")</f>
       </c>
@@ -1859,6 +1983,7 @@
       </c>
       <c r="C126" s="1"/>
       <c r="F126" s="1"/>
+      <c r="H126" s="1"/>
       <c r="J126" s="1">
         <f>IF(F126&lt;&gt;"", "Kg CO2e/" &amp; F126, "")</f>
       </c>
@@ -1870,6 +1995,7 @@
       </c>
       <c r="C127" s="1"/>
       <c r="F127" s="1"/>
+      <c r="H127" s="1"/>
       <c r="J127" s="1">
         <f>IF(F127&lt;&gt;"", "Kg CO2e/" &amp; F127, "")</f>
       </c>
@@ -1881,6 +2007,7 @@
       </c>
       <c r="C128" s="1"/>
       <c r="F128" s="1"/>
+      <c r="H128" s="1"/>
       <c r="J128" s="1">
         <f>IF(F128&lt;&gt;"", "Kg CO2e/" &amp; F128, "")</f>
       </c>
@@ -1892,6 +2019,7 @@
       </c>
       <c r="C129" s="1"/>
       <c r="F129" s="1"/>
+      <c r="H129" s="1"/>
       <c r="J129" s="1">
         <f>IF(F129&lt;&gt;"", "Kg CO2e/" &amp; F129, "")</f>
       </c>
@@ -1903,6 +2031,7 @@
       </c>
       <c r="C130" s="1"/>
       <c r="F130" s="1"/>
+      <c r="H130" s="1"/>
       <c r="J130" s="1">
         <f>IF(F130&lt;&gt;"", "Kg CO2e/" &amp; F130, "")</f>
       </c>
@@ -1914,6 +2043,7 @@
       </c>
       <c r="C131" s="1"/>
       <c r="F131" s="1"/>
+      <c r="H131" s="1"/>
       <c r="J131" s="1">
         <f>IF(F131&lt;&gt;"", "Kg CO2e/" &amp; F131, "")</f>
       </c>
@@ -1925,6 +2055,7 @@
       </c>
       <c r="C132" s="1"/>
       <c r="F132" s="1"/>
+      <c r="H132" s="1"/>
       <c r="J132" s="1">
         <f>IF(F132&lt;&gt;"", "Kg CO2e/" &amp; F132, "")</f>
       </c>
@@ -1936,6 +2067,7 @@
       </c>
       <c r="C133" s="1"/>
       <c r="F133" s="1"/>
+      <c r="H133" s="1"/>
       <c r="J133" s="1">
         <f>IF(F133&lt;&gt;"", "Kg CO2e/" &amp; F133, "")</f>
       </c>
@@ -1947,6 +2079,7 @@
       </c>
       <c r="C134" s="1"/>
       <c r="F134" s="1"/>
+      <c r="H134" s="1"/>
       <c r="J134" s="1">
         <f>IF(F134&lt;&gt;"", "Kg CO2e/" &amp; F134, "")</f>
       </c>
@@ -1958,6 +2091,7 @@
       </c>
       <c r="C135" s="1"/>
       <c r="F135" s="1"/>
+      <c r="H135" s="1"/>
       <c r="J135" s="1">
         <f>IF(F135&lt;&gt;"", "Kg CO2e/" &amp; F135, "")</f>
       </c>
@@ -1969,6 +2103,7 @@
       </c>
       <c r="C136" s="1"/>
       <c r="F136" s="1"/>
+      <c r="H136" s="1"/>
       <c r="J136" s="1">
         <f>IF(F136&lt;&gt;"", "Kg CO2e/" &amp; F136, "")</f>
       </c>
@@ -1980,6 +2115,7 @@
       </c>
       <c r="C137" s="1"/>
       <c r="F137" s="1"/>
+      <c r="H137" s="1"/>
       <c r="J137" s="1">
         <f>IF(F137&lt;&gt;"", "Kg CO2e/" &amp; F137, "")</f>
       </c>
@@ -1991,6 +2127,7 @@
       </c>
       <c r="C138" s="1"/>
       <c r="F138" s="1"/>
+      <c r="H138" s="1"/>
       <c r="J138" s="1">
         <f>IF(F138&lt;&gt;"", "Kg CO2e/" &amp; F138, "")</f>
       </c>
@@ -2002,6 +2139,7 @@
       </c>
       <c r="C139" s="1"/>
       <c r="F139" s="1"/>
+      <c r="H139" s="1"/>
       <c r="J139" s="1">
         <f>IF(F139&lt;&gt;"", "Kg CO2e/" &amp; F139, "")</f>
       </c>
@@ -2013,6 +2151,7 @@
       </c>
       <c r="C140" s="1"/>
       <c r="F140" s="1"/>
+      <c r="H140" s="1"/>
       <c r="J140" s="1">
         <f>IF(F140&lt;&gt;"", "Kg CO2e/" &amp; F140, "")</f>
       </c>
@@ -2024,6 +2163,7 @@
       </c>
       <c r="C141" s="1"/>
       <c r="F141" s="1"/>
+      <c r="H141" s="1"/>
       <c r="J141" s="1">
         <f>IF(F141&lt;&gt;"", "Kg CO2e/" &amp; F141, "")</f>
       </c>
@@ -2035,6 +2175,7 @@
       </c>
       <c r="C142" s="1"/>
       <c r="F142" s="1"/>
+      <c r="H142" s="1"/>
       <c r="J142" s="1">
         <f>IF(F142&lt;&gt;"", "Kg CO2e/" &amp; F142, "")</f>
       </c>
@@ -2046,6 +2187,7 @@
       </c>
       <c r="C143" s="1"/>
       <c r="F143" s="1"/>
+      <c r="H143" s="1"/>
       <c r="J143" s="1">
         <f>IF(F143&lt;&gt;"", "Kg CO2e/" &amp; F143, "")</f>
       </c>
@@ -2057,6 +2199,7 @@
       </c>
       <c r="C144" s="1"/>
       <c r="F144" s="1"/>
+      <c r="H144" s="1"/>
       <c r="J144" s="1">
         <f>IF(F144&lt;&gt;"", "Kg CO2e/" &amp; F144, "")</f>
       </c>
@@ -2068,6 +2211,7 @@
       </c>
       <c r="C145" s="1"/>
       <c r="F145" s="1"/>
+      <c r="H145" s="1"/>
       <c r="J145" s="1">
         <f>IF(F145&lt;&gt;"", "Kg CO2e/" &amp; F145, "")</f>
       </c>
@@ -2079,6 +2223,7 @@
       </c>
       <c r="C146" s="1"/>
       <c r="F146" s="1"/>
+      <c r="H146" s="1"/>
       <c r="J146" s="1">
         <f>IF(F146&lt;&gt;"", "Kg CO2e/" &amp; F146, "")</f>
       </c>
@@ -2090,6 +2235,7 @@
       </c>
       <c r="C147" s="1"/>
       <c r="F147" s="1"/>
+      <c r="H147" s="1"/>
       <c r="J147" s="1">
         <f>IF(F147&lt;&gt;"", "Kg CO2e/" &amp; F147, "")</f>
       </c>
@@ -2101,6 +2247,7 @@
       </c>
       <c r="C148" s="1"/>
       <c r="F148" s="1"/>
+      <c r="H148" s="1"/>
       <c r="J148" s="1">
         <f>IF(F148&lt;&gt;"", "Kg CO2e/" &amp; F148, "")</f>
       </c>
@@ -2112,6 +2259,7 @@
       </c>
       <c r="C149" s="1"/>
       <c r="F149" s="1"/>
+      <c r="H149" s="1"/>
       <c r="J149" s="1">
         <f>IF(F149&lt;&gt;"", "Kg CO2e/" &amp; F149, "")</f>
       </c>
@@ -2123,6 +2271,7 @@
       </c>
       <c r="C150" s="1"/>
       <c r="F150" s="1"/>
+      <c r="H150" s="1"/>
       <c r="J150" s="1">
         <f>IF(F150&lt;&gt;"", "Kg CO2e/" &amp; F150, "")</f>
       </c>
@@ -2134,6 +2283,7 @@
       </c>
       <c r="C151" s="1"/>
       <c r="F151" s="1"/>
+      <c r="H151" s="1"/>
       <c r="J151" s="1">
         <f>IF(F151&lt;&gt;"", "Kg CO2e/" &amp; F151, "")</f>
       </c>
@@ -2145,6 +2295,7 @@
       </c>
       <c r="C152" s="1"/>
       <c r="F152" s="1"/>
+      <c r="H152" s="1"/>
       <c r="J152" s="1">
         <f>IF(F152&lt;&gt;"", "Kg CO2e/" &amp; F152, "")</f>
       </c>
@@ -2156,6 +2307,7 @@
       </c>
       <c r="C153" s="1"/>
       <c r="F153" s="1"/>
+      <c r="H153" s="1"/>
       <c r="J153" s="1">
         <f>IF(F153&lt;&gt;"", "Kg CO2e/" &amp; F153, "")</f>
       </c>
@@ -2167,6 +2319,7 @@
       </c>
       <c r="C154" s="1"/>
       <c r="F154" s="1"/>
+      <c r="H154" s="1"/>
       <c r="J154" s="1">
         <f>IF(F154&lt;&gt;"", "Kg CO2e/" &amp; F154, "")</f>
       </c>
@@ -2178,6 +2331,7 @@
       </c>
       <c r="C155" s="1"/>
       <c r="F155" s="1"/>
+      <c r="H155" s="1"/>
       <c r="J155" s="1">
         <f>IF(F155&lt;&gt;"", "Kg CO2e/" &amp; F155, "")</f>
       </c>
@@ -2189,6 +2343,7 @@
       </c>
       <c r="C156" s="1"/>
       <c r="F156" s="1"/>
+      <c r="H156" s="1"/>
       <c r="J156" s="1">
         <f>IF(F156&lt;&gt;"", "Kg CO2e/" &amp; F156, "")</f>
       </c>
@@ -2200,6 +2355,7 @@
       </c>
       <c r="C157" s="1"/>
       <c r="F157" s="1"/>
+      <c r="H157" s="1"/>
       <c r="J157" s="1">
         <f>IF(F157&lt;&gt;"", "Kg CO2e/" &amp; F157, "")</f>
       </c>
@@ -2211,6 +2367,7 @@
       </c>
       <c r="C158" s="1"/>
       <c r="F158" s="1"/>
+      <c r="H158" s="1"/>
       <c r="J158" s="1">
         <f>IF(F158&lt;&gt;"", "Kg CO2e/" &amp; F158, "")</f>
       </c>
@@ -2227,6 +2384,7 @@
       <c r="F160" s="1">
         <v>1</v>
       </c>
+      <c r="H160" s="1"/>
       <c r="J160" s="1">
         <f>IF(F160&lt;&gt;"", "Kg CO2e/" &amp; F160, "")</f>
       </c>
@@ -3071,7 +3229,7 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <autoFilter ref="A1:F158"/>
-  <dataValidations count="3">
+  <dataValidations count="6">
     <dataValidation type="list" showErrorMessage="1" errorTitle="Invalid Entry" error="Please select a valid unit." sqref="F10:F158">
       <formula1>"Kg,Tonnes,Litres,AED"</formula1>
     </dataValidation>
@@ -3081,6 +3239,15 @@
     <dataValidation type="list" showErrorMessage="1" errorTitle="Invalid Entry" error="Please select a valid unit." sqref="F2:F158">
       <formula1>"Kg,Tonnes,Litres,AED"</formula1>
     </dataValidation>
+    <dataValidation type="list" showErrorMessage="1" errorTitle="Invalid Entry" error="Please select a valid vendor." sqref="H10:H158">
+      <formula1>"SW Jewellery,JK Jewellers,JK Cement"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showErrorMessage="1" errorTitle="Invalid Entry" error="Please select a valid vendor." sqref="H160">
+      <formula1>"SW Jewellery,JK Jewellers,JK Cement"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showErrorMessage="1" errorTitle="Invalid Entry" error="Please select a valid vendor." sqref="H2:H158">
+      <formula1>"SW Jewellery,JK Jewellers,JK Cement"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>

</xml_diff>